<commit_message>
Full human response to plausibility check complete
</commit_message>
<xml_diff>
--- a/coding_batches/batch7/batch7_human_examination_of_final_production_plausibility_check.xlsx
+++ b/coding_batches/batch7/batch7_human_examination_of_final_production_plausibility_check.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benke\devEnv\llmproc\coding_batches\batch7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD326BB-76C7-41D9-9B7F-E1EA7CE732F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A584A174-F494-4A4B-B9DC-082356A7C492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1356" yWindow="-108" windowWidth="21792" windowHeight="14616" xr2:uid="{25318600-D2D6-440C-B8B8-BB886812CC04}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10686" uniqueCount="1706">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10705" uniqueCount="1725">
   <si>
     <t>ID</t>
   </si>
@@ -5138,9 +5138,6 @@
     <t>check failed - There is a significant inconsistency in the article regarding what substance was used. The English Heritage spokeswoman is quoted as saying "Orange powdered paint has been thrown at a number of the stones" while Just Stop Oil's statement claims they "used orange cornflour paint to spray onto the stones." Additionally, the headline and early text refer to "spray paint" while later the article mentions both "powdered paint" and "cornflour paint." This creates confusion about the actual nature of the substance used and appears to be a result of incomplete editing during the article processing.</t>
   </si>
   <si>
-    <t>HUMAN_ASSESSMENT_PLAUSIBILITY_CHECK</t>
-  </si>
-  <si>
     <t>2 - Needs examining</t>
   </si>
   <si>
@@ -5150,7 +5147,67 @@
     <t>0 - Comedy</t>
   </si>
   <si>
-    <t>HUMAN_RESPONSE_TO_PLAUSIBILITY_CHECK</t>
+    <t>HUMAN_FIRST_ASSESSMENT_PLAUSIBILITY_CHECK</t>
+  </si>
+  <si>
+    <t>Real issue. Needs LLM resummary to bring in Dale Vince.</t>
+  </si>
+  <si>
+    <t>No action needed. Phrasing was present in original.</t>
+  </si>
+  <si>
+    <t>HUMAN_FULL_RESPONSE_TO_PLAUSIBILITY_CHECK</t>
+  </si>
+  <si>
+    <t>No action  needed. These articles about revenge actions are potential confusing because they mention two similar actions, but (a) the summarised version is hardly more confusing that the original and (b) minor confusion is unimportant in the context.</t>
+  </si>
+  <si>
+    <t>No action needed. The caption is as in the original and nothing here is particularly confusing or more confusing than in the original.</t>
+  </si>
+  <si>
+    <t>No action needed. The quote is in fact reproduced in full exactly as in original. I think the LLM got confused because the quote is broken up by an image.</t>
+  </si>
+  <si>
+    <t>No action needed. Some of this is just a non-issue, and whereas it's true it's unclear how Plummer's speech was accessed, this is true of the original.</t>
+  </si>
+  <si>
+    <t>No action needed. (1) Same as original. (2) Not that bad and same as original. (3) The summary does jump more abruptly than the original but nothing can be done at this word count and it's OK, I think. (4) Same as original.</t>
+  </si>
+  <si>
+    <t>Real issue. (1) Same as original. (2) Same as original. (3) Easy to reinsert relevant setence at end ("On Thin Ice: Putin v Greenpeace starts on tomorrow, BBC Two at 9pm." so I will).</t>
+  </si>
+  <si>
+    <t>No action needed. Same as original.</t>
+  </si>
+  <si>
+    <t>Eventual action possibly needed, because LLM image description is badly wrong (the gantry is not collapsed), but does not effect article if you don't look at alt-text.</t>
+  </si>
+  <si>
+    <t>No action needed. It is indeed weird that a picture of Chris Martin has a caption that begins with "Dale Vince" but this is what the original does.</t>
+  </si>
+  <si>
+    <t>See response to Mirror_2024-09-27_Just-Stop-Oil-protestors which raises near identical issues.</t>
+  </si>
+  <si>
+    <t>No action needed. For issue of general confusingness, see response to Mirror_2024-09-27_Just-Stop-Oil-protestors which raises near identical issues. Further, it is indeed true that it is odd to say "while the protesters were still attached to the wall" without having said that they glued themselves, but this problem is present in the original.</t>
+  </si>
+  <si>
+    <t>No action needed. I think the LLM is just responding to the fact that the image from Cambridge is positioned nearer to text mentions of Leeds than to mentions of Cambridge, which is no problem.</t>
+  </si>
+  <si>
+    <t>No action needed. LLM being surprisingly gender-normative here, and in fact this is anyway the original article, not a summary.</t>
+  </si>
+  <si>
+    <t>No action needed. LLM being surprisingly gender-normative here, and no issues present not present in original.</t>
+  </si>
+  <si>
+    <t>Real issue. I have been correcting such things when I notice them, so I'll correct this.</t>
+  </si>
+  <si>
+    <t>No action needed. Issue present in original; a real issue, but falls just the wrong side of my threshold on the typo vs stylistic issue continuum (I correct the former but not the latter).</t>
+  </si>
+  <si>
+    <t>Eventual action possibly needed, because LLM image description has failed to OCR the banner, but does not effect article if you don't look at alt-text.</t>
   </si>
 </sst>
 </file>
@@ -5634,11 +5691,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -6014,20 +6072,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AF57DD4-B338-45BC-A77F-5939E4CECC5B}">
-  <dimension ref="A1:Z528"/>
+  <dimension ref="A1:Y528"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="V1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="W1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Y20" sqref="Y20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="46" customWidth="1"/>
+    <col min="1" max="1" width="39.5546875" customWidth="1"/>
     <col min="23" max="23" width="97.33203125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="18.109375" customWidth="1"/>
+    <col min="25" max="25" width="36.77734375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6098,13 +6158,13 @@
         <v>22</v>
       </c>
       <c r="X1" t="s">
-        <v>1701</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>1705</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+        <v>1704</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>245</v>
       </c>
@@ -6169,10 +6229,13 @@
         <v>248</v>
       </c>
       <c r="X2" t="s">
-        <v>1702</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+        <v>1701</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>210</v>
       </c>
@@ -6240,10 +6303,13 @@
         <v>214</v>
       </c>
       <c r="X3" t="s">
-        <v>1702</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+        <v>1701</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>1706</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>423</v>
       </c>
@@ -6314,10 +6380,13 @@
         <v>428</v>
       </c>
       <c r="X4" t="s">
-        <v>1702</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+        <v>1701</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>1708</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>353</v>
       </c>
@@ -6382,10 +6451,13 @@
         <v>356</v>
       </c>
       <c r="X5" t="s">
-        <v>1702</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="86.4" x14ac:dyDescent="0.3">
+        <v>1701</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>1709</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1098</v>
       </c>
@@ -6453,10 +6525,13 @@
         <v>1102</v>
       </c>
       <c r="X6" t="s">
-        <v>1702</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="86.4" x14ac:dyDescent="0.3">
+        <v>1701</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>1710</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1103</v>
       </c>
@@ -6527,10 +6602,13 @@
         <v>1107</v>
       </c>
       <c r="X7" t="s">
-        <v>1702</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="100.8" x14ac:dyDescent="0.3">
+        <v>1701</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>1711</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1631</v>
       </c>
@@ -6598,10 +6676,13 @@
         <v>1634</v>
       </c>
       <c r="X8" t="s">
-        <v>1702</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="86.4" x14ac:dyDescent="0.3">
+        <v>1701</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>1717</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>831</v>
       </c>
@@ -6672,10 +6753,13 @@
         <v>836</v>
       </c>
       <c r="X9" t="s">
-        <v>1702</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="86.4" x14ac:dyDescent="0.3">
+        <v>1701</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>1712</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>876</v>
       </c>
@@ -6746,10 +6830,13 @@
         <v>881</v>
       </c>
       <c r="X10" t="s">
-        <v>1702</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
+        <v>1701</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>1713</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>925</v>
       </c>
@@ -6814,10 +6901,13 @@
         <v>928</v>
       </c>
       <c r="X11" t="s">
-        <v>1702</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
+        <v>1701</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1063</v>
       </c>
@@ -6885,10 +6975,13 @@
         <v>1067</v>
       </c>
       <c r="X12" t="s">
-        <v>1702</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
+        <v>1701</v>
+      </c>
+      <c r="Y12" s="1" t="s">
+        <v>1715</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>537</v>
       </c>
@@ -6953,10 +7046,13 @@
         <v>540</v>
       </c>
       <c r="X13" t="s">
-        <v>1702</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="144" x14ac:dyDescent="0.3">
+        <v>1701</v>
+      </c>
+      <c r="Y13" s="1" t="s">
+        <v>1716</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" ht="144" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>258</v>
       </c>
@@ -7027,10 +7123,13 @@
         <v>264</v>
       </c>
       <c r="X14" t="s">
-        <v>1702</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="86.4" x14ac:dyDescent="0.3">
+        <v>1701</v>
+      </c>
+      <c r="Y14" s="1" t="s">
+        <v>1718</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>1309</v>
       </c>
@@ -7098,10 +7197,13 @@
         <v>1313</v>
       </c>
       <c r="X15" t="s">
-        <v>1702</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
+        <v>1701</v>
+      </c>
+      <c r="Y15" s="1" t="s">
+        <v>1719</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>664</v>
       </c>
@@ -7169,10 +7271,13 @@
         <v>667</v>
       </c>
       <c r="X16" t="s">
-        <v>1702</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+        <v>1701</v>
+      </c>
+      <c r="Y16" s="1" t="s">
+        <v>1720</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>911</v>
       </c>
@@ -7240,10 +7345,13 @@
         <v>915</v>
       </c>
       <c r="X17" t="s">
-        <v>1702</v>
-      </c>
-    </row>
-    <row r="18" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
+        <v>1701</v>
+      </c>
+      <c r="Y17" s="1" t="s">
+        <v>1721</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>1195</v>
       </c>
@@ -7308,10 +7416,13 @@
         <v>1198</v>
       </c>
       <c r="X18" t="s">
-        <v>1702</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+        <v>1701</v>
+      </c>
+      <c r="Y18" s="1" t="s">
+        <v>1722</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>1260</v>
       </c>
@@ -7376,10 +7487,13 @@
         <v>1263</v>
       </c>
       <c r="X19" t="s">
-        <v>1702</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
+        <v>1701</v>
+      </c>
+      <c r="Y19" s="1" t="s">
+        <v>1723</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>1317</v>
       </c>
@@ -7447,10 +7561,13 @@
         <v>1320</v>
       </c>
       <c r="X20" t="s">
-        <v>1702</v>
-      </c>
-    </row>
-    <row r="21" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
+        <v>1701</v>
+      </c>
+      <c r="Y20" s="1" t="s">
+        <v>1724</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>1206</v>
       </c>
@@ -7518,10 +7635,10 @@
         <v>1209</v>
       </c>
       <c r="X21" t="s">
-        <v>1703</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
+        <v>1702</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>191</v>
       </c>
@@ -7586,10 +7703,10 @@
         <v>194</v>
       </c>
       <c r="X22" t="s">
-        <v>1703</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+        <v>1702</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" ht="72" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>955</v>
       </c>
@@ -7657,10 +7774,10 @@
         <v>958</v>
       </c>
       <c r="X23" t="s">
-        <v>1703</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+        <v>1702</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>1492</v>
       </c>
@@ -7728,10 +7845,10 @@
         <v>1495</v>
       </c>
       <c r="X24" t="s">
-        <v>1703</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+        <v>1702</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" ht="72" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>1270</v>
       </c>
@@ -7796,10 +7913,10 @@
         <v>1273</v>
       </c>
       <c r="X25" t="s">
-        <v>1703</v>
-      </c>
-    </row>
-    <row r="26" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
+        <v>1702</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>1011</v>
       </c>
@@ -7867,10 +7984,10 @@
         <v>1015</v>
       </c>
       <c r="X26" t="s">
-        <v>1703</v>
-      </c>
-    </row>
-    <row r="27" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
+        <v>1702</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>504</v>
       </c>
@@ -7941,10 +8058,10 @@
         <v>509</v>
       </c>
       <c r="X27" t="s">
-        <v>1703</v>
-      </c>
-    </row>
-    <row r="28" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+        <v>1702</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" ht="72" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>989</v>
       </c>
@@ -8012,10 +8129,10 @@
         <v>992</v>
       </c>
       <c r="X28" t="s">
-        <v>1703</v>
-      </c>
-    </row>
-    <row r="29" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+        <v>1702</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>1697</v>
       </c>
@@ -8083,10 +8200,10 @@
         <v>1700</v>
       </c>
       <c r="X29" t="s">
-        <v>1703</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+        <v>1702</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" ht="72" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>72</v>
       </c>
@@ -8154,10 +8271,10 @@
         <v>77</v>
       </c>
       <c r="X30" t="s">
-        <v>1703</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
+        <v>1702</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -8225,10 +8342,10 @@
         <v>38</v>
       </c>
       <c r="X31" t="s">
-        <v>1703</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+        <v>1702</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" ht="72" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>330</v>
       </c>
@@ -8299,7 +8416,7 @@
         <v>334</v>
       </c>
       <c r="X32" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
     </row>
     <row r="33" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
@@ -8370,7 +8487,7 @@
         <v>1202</v>
       </c>
       <c r="X33" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
     </row>
     <row r="34" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
@@ -8441,7 +8558,7 @@
         <v>1687</v>
       </c>
       <c r="X34" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
     </row>
     <row r="35" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
@@ -8509,7 +8626,7 @@
         <v>103</v>
       </c>
       <c r="X35" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
     </row>
     <row r="36" spans="1:24" ht="72" x14ac:dyDescent="0.3">
@@ -8577,7 +8694,7 @@
         <v>84</v>
       </c>
       <c r="X36" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
     </row>
     <row r="37" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
@@ -8648,7 +8765,7 @@
         <v>559</v>
       </c>
       <c r="X37" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.3">

</xml_diff>